<commit_message>
Item, Weapon, Armor, Consumable DB 추가
Item, Weapon, Armor, Consumable DB 추가 및 데이터 컴포넌트 구현
</commit_message>
<xml_diff>
--- a/Assets/DataTables/CharacterDB.xlsx
+++ b/Assets/DataTables/CharacterDB.xlsx
@@ -37,7 +37,7 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Str:+10;Dex:+20;Luck:+30;Int:-40;</t>
+    <t>HP:+100;SP:+100;Str:+10;Dex:+20;Luck:+30;Int:-40;</t>
   </si>
 </sst>
 </file>
@@ -313,7 +313,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1.0000001E7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
CharacterData 읽어서 WeaponData 값 적용하는 로직 추가
CharacterData 읽어서 WeaponData 값 적용하는 로직 추가
</commit_message>
<xml_diff>
--- a/Assets/DataTables/CharacterDB.xlsx
+++ b/Assets/DataTables/CharacterDB.xlsx
@@ -19,13 +19,13 @@
     <t>Type</t>
   </si>
   <si>
-    <t>DefaultName</t>
-  </si>
-  <si>
-    <t>DefaultGender</t>
-  </si>
-  <si>
-    <t>DefaultStat</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Stat</t>
   </si>
   <si>
     <t>PC</t>

</xml_diff>